<commit_message>
completed carbon materials debug
it all works, was just math in the testing file that was sloppy. User or in aggregate results needs to remember to add LQ and HQ recycling together
</commit_message>
<xml_diff>
--- a/PV_ICE/baselines/SupportingMaterial/CarbonIntensities/Dummy_test.xlsx
+++ b/PV_ICE/baselines/SupportingMaterial/CarbonIntensities/Dummy_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmirletz\Documents\GitHub\PV_ICE\PV_ICE\baselines\SupportingMaterial\CarbonIntensities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8EB17F-5256-4857-8DBF-F25862BDA508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A08C9E1-1BCD-44E2-9E10-6F0D1786C6EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9700" yWindow="350" windowWidth="14250" windowHeight="11060" xr2:uid="{1347AB27-8724-4A04-A5D9-957BB6E10CF0}"/>
+    <workbookView xWindow="47640" yWindow="-6285" windowWidth="9900" windowHeight="15600" xr2:uid="{1347AB27-8724-4A04-A5D9-957BB6E10CF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="87">
   <si>
     <t>MW</t>
   </si>
@@ -71,9 +71,6 @@
     <t>China grid mfg</t>
   </si>
   <si>
-    <t>year</t>
-  </si>
-  <si>
     <t>China_Bioenergy</t>
   </si>
   <si>
@@ -185,9 +182,6 @@
     <t>Ember</t>
   </si>
   <si>
-    <t>fuel fraction of vmfging</t>
-  </si>
-  <si>
     <t>gCO2/gSi</t>
   </si>
   <si>
@@ -197,23 +191,122 @@
     <t xml:space="preserve">gCO2 </t>
   </si>
   <si>
-    <t>Si mfging from China 2050</t>
-  </si>
-  <si>
     <t>Module Dummy Test</t>
   </si>
   <si>
-    <t>vmfging China electricity</t>
-  </si>
-  <si>
     <t>error</t>
+  </si>
+  <si>
+    <t>vmfg material Fuel</t>
+  </si>
+  <si>
+    <t>fuel fraction of vmfging (steam and heat)</t>
+  </si>
+  <si>
+    <t>China_vmfg_elec_gCO2eq</t>
+  </si>
+  <si>
+    <t>gco2eq/Wh</t>
+  </si>
+  <si>
+    <t>carbon intensity of china grid 2050 from code</t>
+  </si>
+  <si>
+    <t>USA_Bioenergy</t>
+  </si>
+  <si>
+    <t>USA_Coal</t>
+  </si>
+  <si>
+    <t>USA_Gas</t>
+  </si>
+  <si>
+    <t>USA_Hydro</t>
+  </si>
+  <si>
+    <t>USA_Nuclear</t>
+  </si>
+  <si>
+    <t>USA_OtherFossil</t>
+  </si>
+  <si>
+    <t>USA_Solar</t>
+  </si>
+  <si>
+    <t>USA_Wind</t>
+  </si>
+  <si>
+    <t>from process emissions of si</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>end of life L0</t>
+  </si>
+  <si>
+    <t>landfill energy (all elec)</t>
+  </si>
+  <si>
+    <t>Landfilling in 2050 in US</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>USA landfilling</t>
+  </si>
+  <si>
+    <t>USA carbon intensity</t>
+  </si>
+  <si>
+    <t>China carbon intensity</t>
+  </si>
+  <si>
+    <t>And now with more recycling</t>
+  </si>
+  <si>
+    <t>from code HQ co2 from electicity of recycling</t>
+  </si>
+  <si>
+    <t>EOL material going to Recycling</t>
+  </si>
+  <si>
+    <t>% fuel</t>
+  </si>
+  <si>
+    <t>Energy of HQ recycling</t>
+  </si>
+  <si>
+    <t>prct fuel of HQ recycling</t>
+  </si>
+  <si>
+    <t>Energy of LQ recycling</t>
+  </si>
+  <si>
+    <t>electricity of recycling</t>
+  </si>
+  <si>
+    <t>CO2eq</t>
+  </si>
+  <si>
+    <t>CO2 emissions from recycling electricity</t>
+  </si>
+  <si>
+    <t>energy of HQ recycling electricity</t>
+  </si>
+  <si>
+    <t>NOTE: the LQ and HQ are not added automatically together</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,13 +334,33 @@
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -343,13 +456,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -362,6 +474,16 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="169" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,22 +799,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D092966F-D309-49B7-A0C3-E87EE47EB71C}">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.08984375" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="10.7265625" customWidth="1"/>
     <col min="3" max="3" width="11.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="11" t="s">
-        <v>54</v>
+      <c r="A1" s="10" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -761,7 +883,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -784,7 +906,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -793,48 +915,48 @@
         <v>21832970.636865806</v>
       </c>
       <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="10">
+      <c r="A11" s="9">
         <f>A10</f>
         <v>21832970.636865806</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="J13" s="3"/>
     </row>
@@ -842,88 +964,88 @@
       <c r="A14" s="4">
         <v>2050</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14">
         <v>2</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14">
         <v>62.93</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14">
         <v>3.21</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14">
         <v>15.32</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14">
         <v>4.8</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14">
         <v>0.14000000000000001</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14">
         <v>3.85</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14">
         <v>7.73</v>
       </c>
-      <c r="J14" s="6"/>
+      <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="D15" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="E15" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="F15" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="G15" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="H15" t="s">
         <v>25</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="I15" t="s">
         <v>26</v>
       </c>
-      <c r="I15" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>47</v>
+      <c r="J15" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="4"/>
-      <c r="B16" s="5">
+      <c r="B16">
         <v>0.23</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16">
         <v>0.82</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16">
         <v>0.49</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16">
         <v>2.4E-2</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16">
         <v>1.2E-2</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16">
         <v>0.7</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H16">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="I16" s="5">
+      <c r="I16">
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="J16">
@@ -931,191 +1053,465 @@
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="7">
+      <c r="A17" s="6">
         <f>SUM(B17:I17)</f>
         <v>0.54428609999999999</v>
       </c>
-      <c r="B17" s="8">
-        <f>B14*B16/100</f>
+      <c r="B17" s="7">
+        <f>(B14/100)*B16</f>
         <v>4.5999999999999999E-3</v>
       </c>
-      <c r="C17" s="8">
-        <f t="shared" ref="C17:I17" si="0">C14*C16/100</f>
+      <c r="C17" s="7">
+        <f t="shared" ref="C17:I17" si="0">(C14/100)*C16</f>
         <v>0.51602599999999998</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="7">
         <f t="shared" si="0"/>
-        <v>1.5729E-2</v>
-      </c>
-      <c r="E17" s="8">
+        <v>1.5728999999999996E-2</v>
+      </c>
+      <c r="E17" s="7">
         <f t="shared" si="0"/>
         <v>3.6768E-3</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="7">
         <f t="shared" si="0"/>
         <v>5.7600000000000001E-4</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="7">
         <f t="shared" si="0"/>
-        <v>9.7999999999999997E-4</v>
-      </c>
-      <c r="H17" s="8">
+        <v>9.8000000000000019E-4</v>
+      </c>
+      <c r="H17" s="7">
         <f t="shared" si="0"/>
-        <v>1.8480000000000003E-3</v>
-      </c>
-      <c r="I17" s="8">
+        <v>1.848E-3</v>
+      </c>
+      <c r="I17" s="7">
         <f t="shared" si="0"/>
-        <v>8.5029999999999991E-4</v>
-      </c>
-      <c r="J17" s="9"/>
+        <v>8.5030000000000001E-4</v>
+      </c>
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" t="s">
+        <v>63</v>
+      </c>
+      <c r="H18" t="s">
+        <v>64</v>
+      </c>
+      <c r="I18" t="s">
+        <v>65</v>
+      </c>
+      <c r="J18" s="14"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19">
+        <v>2050</v>
+      </c>
+      <c r="B19">
+        <v>10.79</v>
+      </c>
+      <c r="C19">
+        <v>1.61</v>
+      </c>
+      <c r="D19">
+        <v>39.26</v>
+      </c>
+      <c r="E19">
+        <v>1.76</v>
+      </c>
+      <c r="F19">
+        <v>14.82</v>
+      </c>
+      <c r="G19">
+        <v>2.86</v>
+      </c>
+      <c r="H19">
+        <v>4.28</v>
+      </c>
+      <c r="I19">
+        <v>24.62</v>
+      </c>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21">
-        <v>100</v>
-      </c>
-      <c r="B21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" t="s">
-        <v>35</v>
+      <c r="A20" s="6">
+        <f>SUM(B20:I20)</f>
+        <v>0.25737640000000001</v>
+      </c>
+      <c r="B20" s="7">
+        <f>(B19/100)*B16</f>
+        <v>2.4816999999999999E-2</v>
+      </c>
+      <c r="C20" s="7">
+        <f t="shared" ref="C20:I20" si="1">(C19/100)*C16</f>
+        <v>1.3201999999999998E-2</v>
+      </c>
+      <c r="D20" s="7">
+        <f t="shared" si="1"/>
+        <v>0.19237399999999999</v>
+      </c>
+      <c r="E20" s="7">
+        <f t="shared" si="1"/>
+        <v>4.2240000000000002E-4</v>
+      </c>
+      <c r="F20" s="7">
+        <f t="shared" si="1"/>
+        <v>1.7784000000000001E-3</v>
+      </c>
+      <c r="G20" s="7">
+        <f t="shared" si="1"/>
+        <v>2.002E-2</v>
+      </c>
+      <c r="H20" s="7">
+        <f t="shared" si="1"/>
+        <v>2.0544000000000001E-3</v>
+      </c>
+      <c r="I20" s="7">
+        <f t="shared" si="1"/>
+        <v>2.7082E-3</v>
       </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22">
-        <f>A21*A5</f>
-        <v>50000000</v>
-      </c>
-      <c r="B22" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" t="s">
-        <v>42</v>
+      <c r="A22" s="10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24">
-        <v>50</v>
+        <f>A23*A5</f>
+        <v>50000000</v>
       </c>
       <c r="B24" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="C24" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25">
-        <f>A23*A22</f>
-        <v>50000000</v>
+        <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26">
-        <v>84.094991329999999</v>
+        <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27">
-        <f>A25*(A24/100)*A9*(A26/100)</f>
-        <v>9180217.3820768725</v>
+        <f>A25*A24</f>
+        <v>50000000</v>
       </c>
       <c r="B27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28">
+        <f>A27*(A26/100)</f>
+        <v>25000000</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29">
+        <v>84.094991329999999</v>
+      </c>
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="11">
+        <f>A17*(A29/100)</f>
+        <v>0.45771734860539515</v>
+      </c>
+      <c r="B30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="16">
+        <f>(A27-A28)*A30</f>
+        <v>11442933.71513488</v>
+      </c>
+      <c r="B31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" t="s">
         <v>45</v>
       </c>
-      <c r="C27" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="12">
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="13">
         <v>11442933.715134799</v>
-      </c>
-      <c r="B28" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="13">
-        <f>(A28-A27)/A28</f>
-        <v>0.19773918029999457</v>
-      </c>
-      <c r="B29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="12"/>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="A31">
-        <f>(A24/100)*A25*J16</f>
-        <v>5665000</v>
-      </c>
-      <c r="B31" t="s">
-        <v>45</v>
-      </c>
-      <c r="C31" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32">
-        <v>5.0330000000000004</v>
       </c>
       <c r="B32" t="s">
         <v>50</v>
       </c>
       <c r="C32" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33">
-        <f>A32*A22</f>
+      <c r="A33" s="12">
+        <f>(A32-A31)/A32</f>
+        <v>-6.9994062196652017E-15</v>
+      </c>
+      <c r="B33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="11"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="15">
+        <f>A28*J16</f>
+        <v>5665000</v>
+      </c>
+      <c r="B35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37">
+        <v>5.0330000000000004</v>
+      </c>
+      <c r="B37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="15">
+        <f>A37*A24</f>
         <v>251650000.00000003</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35">
-        <f>SUM(A27:A32)</f>
-        <v>26288156.327950854</v>
-      </c>
-      <c r="B35" t="s">
-        <v>52</v>
-      </c>
-      <c r="C35" t="s">
-        <v>53</v>
+      <c r="B38" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40">
+        <v>50000000</v>
+      </c>
+      <c r="B40" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41" t="s">
+        <v>35</v>
+      </c>
+      <c r="C41" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42">
+        <f>A40*A41</f>
+        <v>50000000</v>
+      </c>
+      <c r="B42" t="s">
+        <v>39</v>
+      </c>
+      <c r="C42" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="15">
+        <f>A42*A20</f>
+        <v>12868820</v>
+      </c>
+      <c r="B43" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="17">
+        <v>12868820</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="17">
+        <v>6434410</v>
+      </c>
+      <c r="B47" t="s">
+        <v>83</v>
+      </c>
+      <c r="C47" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48">
+        <f>A47/A20</f>
+        <v>25000000</v>
+      </c>
+      <c r="B48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49">
+        <v>50000000</v>
+      </c>
+      <c r="B49" t="s">
+        <v>67</v>
+      </c>
+      <c r="C49" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="18">
+        <v>1</v>
+      </c>
+      <c r="B50" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51" t="s">
+        <v>35</v>
+      </c>
+      <c r="C51" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53">
+        <f>A51*(A52/100)</f>
+        <v>0.5</v>
+      </c>
+      <c r="B53" t="s">
+        <v>35</v>
+      </c>
+      <c r="C53" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54">
+        <f>A49*(A53)</f>
+        <v>25000000</v>
+      </c>
+      <c r="B54" t="s">
+        <v>39</v>
+      </c>
+      <c r="C54" t="s">
+        <v>82</v>
+      </c>
+      <c r="E54" s="18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55">
+        <f>A54*A20</f>
+        <v>6434410</v>
+      </c>
+      <c r="B55" t="s">
+        <v>83</v>
+      </c>
+      <c r="C55" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>